<commit_message>
Fixed typo in Stories_Activities.xlsx
</commit_message>
<xml_diff>
--- a/Gallery/Stories_Activities.xlsx
+++ b/Gallery/Stories_Activities.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_1F7B85D8DEA5EB7B84D30F5027211B338BD6DF0A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8AA4722-107D-452B-AAB8-46B00699F17D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>AnnaLearns-WhoIsWho.el</t>
   </si>
@@ -226,12 +227,15 @@
   </si>
   <si>
     <t>HauntedHouse.pt</t>
+  </si>
+  <si>
+    <t>HauntedHouse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -288,18 +292,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -581,11 +584,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +598,6 @@
     <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="37" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -614,38 +616,38 @@
       <c r="E1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1"/>
+      <c r="X1"/>
+      <c r="Y1"/>
+      <c r="Z1"/>
+      <c r="AA1"/>
+      <c r="AB1"/>
+      <c r="AC1"/>
+      <c r="AD1"/>
+      <c r="AE1"/>
+      <c r="AF1"/>
+      <c r="AG1"/>
+      <c r="AH1"/>
+      <c r="AI1"/>
+      <c r="AJ1"/>
+      <c r="AK1"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -792,38 +794,38 @@
       <c r="E14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="5"/>
-      <c r="AB14" s="5"/>
-      <c r="AC14" s="5"/>
-      <c r="AD14" s="5"/>
-      <c r="AE14" s="5"/>
-      <c r="AF14" s="5"/>
-      <c r="AG14" s="5"/>
-      <c r="AH14" s="5"/>
-      <c r="AI14" s="5"/>
-      <c r="AJ14" s="5"/>
-      <c r="AK14" s="5"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -842,9 +844,6 @@
       <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -856,7 +855,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
@@ -888,54 +887,54 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:37" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-      <c r="Z24" s="5"/>
-      <c r="AA24" s="5"/>
-      <c r="AB24" s="5"/>
-      <c r="AC24" s="5"/>
-      <c r="AD24" s="5"/>
-      <c r="AE24" s="5"/>
-      <c r="AF24" s="5"/>
-      <c r="AG24" s="5"/>
-      <c r="AH24" s="5"/>
-      <c r="AI24" s="5"/>
-      <c r="AJ24" s="5"/>
-      <c r="AK24" s="5"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+      <c r="Z24"/>
+      <c r="AA24"/>
+      <c r="AB24"/>
+      <c r="AC24"/>
+      <c r="AD24"/>
+      <c r="AE24"/>
+      <c r="AF24"/>
+      <c r="AG24"/>
+      <c r="AH24"/>
+      <c r="AI24"/>
+      <c r="AJ24"/>
+      <c r="AK24"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">

</xml_diff>